<commit_message>
Debuging of output where overflow was present even though release was zero and storage was not maximum.
</commit_message>
<xml_diff>
--- a/Sunkoshi.xlsx
+++ b/Sunkoshi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\OneDrive\Desktop\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46E351B-010D-4A8D-8C0A-C4E39341241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E4F8FA-A917-4400-9215-65D6911110A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="90" windowWidth="20385" windowHeight="10830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUNKOSHI1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Dudhkoshi1!$D$1:$D$76</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SUNKOSHI2!$A$1:$C$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SUNKOSHI2!$A$1:$C$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -106,13 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -463,7 +462,7 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -475,7 +474,7 @@
       <c r="C5" s="1">
         <v>1.85948073</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -487,7 +486,7 @@
       <c r="C6" s="1">
         <v>14.904654730000001</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -499,7 +498,7 @@
       <c r="C7" s="1">
         <v>32.900587059999999</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -511,7 +510,7 @@
       <c r="C8" s="1">
         <v>55.106977409999999</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -523,7 +522,7 @@
       <c r="C9" s="1">
         <v>80.251871120000004</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -535,7 +534,7 @@
       <c r="C10" s="1">
         <v>109.18469295</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -547,7 +546,7 @@
       <c r="C11" s="1">
         <v>142.70859891000001</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -559,7 +558,7 @@
       <c r="C12" s="1">
         <v>183.63725396999999</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -571,7 +570,7 @@
       <c r="C13" s="1">
         <v>231.04179076</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -583,7 +582,7 @@
       <c r="C14" s="1">
         <v>284.92570126999999</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -595,7 +594,7 @@
       <c r="C15" s="1">
         <v>344.50154341000001</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -607,7 +606,7 @@
       <c r="C16" s="1">
         <v>409.57463917000001</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -995,36 +994,36 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1034,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1047,7 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1059,387 +1058,187 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>505</v>
+      </c>
+      <c r="B2" s="8">
+        <v>26525189</v>
       </c>
       <c r="C2" s="2">
         <v>-999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>415</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>505</v>
+      </c>
+      <c r="B3" s="8">
+        <v>26525189</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>420</v>
-      </c>
-      <c r="B4" s="9">
-        <v>95164</v>
+        <v>776.99960099999998</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>510</v>
+      </c>
+      <c r="B4" s="8">
+        <v>28975045</v>
       </c>
       <c r="C4" s="1">
-        <v>0.18609500000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>425</v>
-      </c>
-      <c r="B5" s="9">
-        <v>416500</v>
+        <v>915.70510400000001</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>515</v>
+      </c>
+      <c r="B5" s="8">
+        <v>31464569</v>
       </c>
       <c r="C5" s="1">
-        <v>1.370682</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>430</v>
-      </c>
-      <c r="B6" s="9">
-        <v>666866</v>
+        <v>1066.761393</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>520</v>
+      </c>
+      <c r="B6" s="8">
+        <v>34279689</v>
       </c>
       <c r="C6" s="1">
-        <v>4.0546569999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>435</v>
-      </c>
-      <c r="B7" s="9">
-        <v>972380</v>
+        <v>1231.071788</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>525</v>
+      </c>
+      <c r="B7" s="8">
+        <v>37170299</v>
       </c>
       <c r="C7" s="1">
-        <v>8.1288359999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>440</v>
-      </c>
-      <c r="B8" s="9">
-        <v>1687313</v>
+        <v>1409.6480100000001</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>530</v>
+      </c>
+      <c r="B8" s="8">
+        <v>39748363</v>
       </c>
       <c r="C8" s="1">
-        <v>14.696494</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>445</v>
-      </c>
-      <c r="B9" s="9">
-        <v>2479995</v>
+        <v>1601.908651</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>535</v>
+      </c>
+      <c r="B9" s="8">
+        <v>42257913</v>
       </c>
       <c r="C9" s="1">
-        <v>25.051359999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>450</v>
-      </c>
-      <c r="B10" s="9">
-        <v>3520413</v>
+        <v>1806.8923339999999</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>540</v>
+      </c>
+      <c r="B10" s="8">
+        <v>45163693</v>
       </c>
       <c r="C10" s="1">
-        <v>39.976640000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>455</v>
-      </c>
-      <c r="B11" s="9">
-        <v>4690947</v>
+        <v>2025.4060950000001</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>545</v>
+      </c>
+      <c r="B11" s="8">
+        <v>47944949</v>
       </c>
       <c r="C11" s="1">
-        <v>60.435158000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>460</v>
-      </c>
-      <c r="B12" s="9">
-        <v>6305042</v>
+        <v>2258.1430770000002</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>550</v>
+      </c>
+      <c r="B12" s="8">
+        <v>50685466</v>
       </c>
       <c r="C12" s="1">
-        <v>87.825872000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>465</v>
-      </c>
-      <c r="B13" s="9">
-        <v>7990675</v>
+        <v>2504.687379</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>555</v>
+      </c>
+      <c r="B13" s="8">
+        <v>53262183</v>
       </c>
       <c r="C13" s="1">
-        <v>123.48206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>470</v>
-      </c>
-      <c r="B14" s="9">
-        <v>9725069</v>
+        <v>2764.5298830000002</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>560</v>
+      </c>
+      <c r="B14" s="8">
+        <v>55760323</v>
       </c>
       <c r="C14" s="1">
-        <v>167.700502</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>475</v>
-      </c>
-      <c r="B15" s="9">
-        <v>12091881</v>
-      </c>
-      <c r="C15" s="1">
-        <v>222.13557599999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>480</v>
-      </c>
-      <c r="B16" s="9">
-        <v>13797723</v>
-      </c>
-      <c r="C16" s="1">
-        <v>286.812703</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>485</v>
-      </c>
-      <c r="B17" s="9">
-        <v>15864072</v>
-      </c>
-      <c r="C17" s="1">
-        <v>360.90713799999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>490</v>
-      </c>
-      <c r="B18" s="9">
-        <v>18407881</v>
-      </c>
-      <c r="C18" s="1">
-        <v>446.508239</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>495</v>
-      </c>
-      <c r="B19" s="9">
-        <v>19499842</v>
-      </c>
-      <c r="C19" s="1">
-        <v>541.26443900000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>500</v>
-      </c>
-      <c r="B20" s="9">
-        <v>24185520</v>
-      </c>
-      <c r="C20" s="1">
-        <v>650.26783</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>505</v>
-      </c>
-      <c r="B21" s="9">
-        <v>26525189</v>
-      </c>
-      <c r="C21" s="1">
-        <v>776.99960099999998</v>
-      </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>510</v>
-      </c>
-      <c r="B22" s="9">
-        <v>28975045</v>
-      </c>
-      <c r="C22" s="1">
-        <v>915.70510400000001</v>
-      </c>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>515</v>
-      </c>
-      <c r="B23" s="9">
-        <v>31464569</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1066.761393</v>
-      </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>520</v>
-      </c>
-      <c r="B24" s="9">
-        <v>34279689</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1231.071788</v>
-      </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>525</v>
-      </c>
-      <c r="B25" s="9">
-        <v>37170299</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1409.6480100000001</v>
-      </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>530</v>
-      </c>
-      <c r="B26" s="9">
-        <v>39748363</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1601.908651</v>
-      </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>535</v>
-      </c>
-      <c r="B27" s="9">
-        <v>42257913</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1806.8923339999999</v>
-      </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>540</v>
-      </c>
-      <c r="B28" s="9">
-        <v>45163693</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2025.4060950000001</v>
-      </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>545</v>
-      </c>
-      <c r="B29" s="9">
-        <v>47944949</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2258.1430770000002</v>
-      </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>550</v>
-      </c>
-      <c r="B30" s="9">
-        <v>50685466</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2504.687379</v>
-      </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>555</v>
-      </c>
-      <c r="B31" s="9">
-        <v>53262183</v>
-      </c>
-      <c r="C31" s="1">
-        <v>2764.5298830000002</v>
-      </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
-        <v>560</v>
-      </c>
-      <c r="B32" s="9">
-        <v>55760323</v>
-      </c>
-      <c r="C32" s="1">
         <v>3037.0622939999998</v>
       </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="5"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1451,17 +1250,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1476,10 +1275,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>660</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>18566382</v>
       </c>
       <c r="C2" s="1">
@@ -1487,10 +1286,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>660</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>18566382</v>
       </c>
       <c r="C3" s="1">
@@ -1498,10 +1297,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>665</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>20049720</v>
       </c>
       <c r="C4" s="1">
@@ -1509,10 +1308,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>670</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>21558521</v>
       </c>
       <c r="C5" s="1">
@@ -1520,10 +1319,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>675</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>23092817</v>
       </c>
       <c r="C6" s="1">
@@ -1531,10 +1330,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>680</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>24795233</v>
       </c>
       <c r="C7" s="1">
@@ -1542,10 +1341,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>685</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>26443966</v>
       </c>
       <c r="C8" s="1">
@@ -1553,10 +1352,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>690</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>28282644</v>
       </c>
       <c r="C9" s="1">
@@ -1564,10 +1363,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>695</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>30314696</v>
       </c>
       <c r="C10" s="1">
@@ -1575,10 +1374,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>700</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>32369897</v>
       </c>
       <c r="C11" s="1">
@@ -1586,10 +1385,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>705</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>34525649</v>
       </c>
       <c r="C12" s="1">
@@ -1597,10 +1396,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>710</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>36554536</v>
       </c>
       <c r="C13" s="1">

</xml_diff>

<commit_message>
Added single operation codes for dudhkoshi and sunkoshi 1
</commit_message>
<xml_diff>
--- a/Sunkoshi.xlsx
+++ b/Sunkoshi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\OneDrive\Desktop\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E4F8FA-A917-4400-9215-65D6911110A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17004863-F3E3-411F-9AAE-FBD2FE20452A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUNKOSHI1" sheetId="2" r:id="rId1"/>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
improved empso and changed data file
</commit_message>
<xml_diff>
--- a/Sunkoshi.xlsx
+++ b/Sunkoshi.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\OneDrive\Desktop\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17004863-F3E3-411F-9AAE-FBD2FE20452A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B12B613-048A-4C86-BFA0-7E58B6059DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7290" yWindow="165" windowWidth="20370" windowHeight="10830" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUNKOSHI1" sheetId="2" r:id="rId1"/>
     <sheet name="SUNKOSHI2" sheetId="3" r:id="rId2"/>
     <sheet name="SUNKOSHI3" sheetId="4" r:id="rId3"/>
     <sheet name="Dudhkoshi1" sheetId="5" r:id="rId4"/>
+    <sheet name="Saptakoshi" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Dudhkoshi1!$D$1:$D$76</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
     <t>Vol</t>
   </si>
@@ -408,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A28" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection sqref="A1:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1418,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,4 +1952,2455 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C185D36C-FBE8-4DB7-A721-65612F35B497}">
+  <dimension ref="A1:C221"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="E177" sqref="E177"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>91</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>92</v>
+      </c>
+      <c r="B3">
+        <v>884.13978499999996</v>
+      </c>
+      <c r="C3">
+        <v>8.8413978499999994E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>93</v>
+      </c>
+      <c r="B4">
+        <v>1768.2795699999999</v>
+      </c>
+      <c r="C4">
+        <v>2.6524193549999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>94</v>
+      </c>
+      <c r="B5">
+        <v>4420.6989240000003</v>
+      </c>
+      <c r="C5">
+        <v>7.073118279E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>95</v>
+      </c>
+      <c r="B6">
+        <v>11493.817204000001</v>
+      </c>
+      <c r="C6">
+        <v>1.8566935483000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>96</v>
+      </c>
+      <c r="B7">
+        <v>23871.774192000001</v>
+      </c>
+      <c r="C7">
+        <v>4.2438709674999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>97</v>
+      </c>
+      <c r="B8">
+        <v>34481.451610999997</v>
+      </c>
+      <c r="C8">
+        <v>7.6920161286000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>98</v>
+      </c>
+      <c r="B9">
+        <v>41554.569889999999</v>
+      </c>
+      <c r="C9">
+        <v>0.11847473117600001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>99</v>
+      </c>
+      <c r="B10">
+        <v>53048.387093999998</v>
+      </c>
+      <c r="C10">
+        <v>0.17152311827</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>68078.763437000001</v>
+      </c>
+      <c r="C11">
+        <v>0.239601881707</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>101</v>
+      </c>
+      <c r="B12">
+        <v>90182.258059</v>
+      </c>
+      <c r="C12">
+        <v>0.32978413976599996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>109633.333327</v>
+      </c>
+      <c r="C13">
+        <v>0.439417473093</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>103</v>
+      </c>
+      <c r="B14">
+        <v>141462.36558300001</v>
+      </c>
+      <c r="C14">
+        <v>0.58087983867699999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>104</v>
+      </c>
+      <c r="B15">
+        <v>165334.139776</v>
+      </c>
+      <c r="C15">
+        <v>0.74621397845199999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>105</v>
+      </c>
+      <c r="B16">
+        <v>198931.45160199999</v>
+      </c>
+      <c r="C16">
+        <v>0.94514543005399998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>106</v>
+      </c>
+      <c r="B17">
+        <v>239601.88170699999</v>
+      </c>
+      <c r="C17">
+        <v>1.1847473117609999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>107</v>
+      </c>
+      <c r="B18">
+        <v>270546.77417799999</v>
+      </c>
+      <c r="C18">
+        <v>1.455294085939</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>108</v>
+      </c>
+      <c r="B19">
+        <v>313869.62363799999</v>
+      </c>
+      <c r="C19">
+        <v>1.7691637095770001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>109</v>
+      </c>
+      <c r="B20">
+        <v>357192.47309799999</v>
+      </c>
+      <c r="C20">
+        <v>2.126356182676</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>110</v>
+      </c>
+      <c r="B21">
+        <v>401399.46234299999</v>
+      </c>
+      <c r="C21">
+        <v>2.527755645019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>111</v>
+      </c>
+      <c r="B22">
+        <v>453563.70965199999</v>
+      </c>
+      <c r="C22">
+        <v>2.9813193546699996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>112</v>
+      </c>
+      <c r="B23">
+        <v>503075.53760600003</v>
+      </c>
+      <c r="C23">
+        <v>3.4843948922760002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>113</v>
+      </c>
+      <c r="B24">
+        <v>573806.72039799998</v>
+      </c>
+      <c r="C24">
+        <v>4.0582016126739999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>114</v>
+      </c>
+      <c r="B25">
+        <v>615361.29028800002</v>
+      </c>
+      <c r="C25">
+        <v>4.6735629029619998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>115</v>
+      </c>
+      <c r="B26">
+        <v>678135.21501499997</v>
+      </c>
+      <c r="C26">
+        <v>5.3516981179769996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>116</v>
+      </c>
+      <c r="B27">
+        <v>743561.55909800006</v>
+      </c>
+      <c r="C27">
+        <v>6.0952596770749992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>117</v>
+      </c>
+      <c r="B28">
+        <v>795725.80640700005</v>
+      </c>
+      <c r="C28">
+        <v>6.8909854834820008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>118</v>
+      </c>
+      <c r="B29">
+        <v>863804.56984400004</v>
+      </c>
+      <c r="C29">
+        <v>7.7547900533250003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>119</v>
+      </c>
+      <c r="B30">
+        <v>942493.01069899998</v>
+      </c>
+      <c r="C30">
+        <v>8.6972830640249992</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>120</v>
+      </c>
+      <c r="B31">
+        <v>1030906.989189</v>
+      </c>
+      <c r="C31">
+        <v>9.728190053214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>121</v>
+      </c>
+      <c r="B32">
+        <v>1113131.9891840001</v>
+      </c>
+      <c r="C32">
+        <v>10.841322042398</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>122</v>
+      </c>
+      <c r="B33">
+        <v>1206850.806383</v>
+      </c>
+      <c r="C33">
+        <v>12.048172848781999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>123</v>
+      </c>
+      <c r="B34">
+        <v>1320020.69885</v>
+      </c>
+      <c r="C34">
+        <v>13.368193547632</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>124</v>
+      </c>
+      <c r="B35">
+        <v>1444684.4085210001</v>
+      </c>
+      <c r="C35">
+        <v>14.812877956153001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>125</v>
+      </c>
+      <c r="B36">
+        <v>1554317.7418480001</v>
+      </c>
+      <c r="C36">
+        <v>16.367195698</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>126</v>
+      </c>
+      <c r="B37">
+        <v>1673676.6128090001</v>
+      </c>
+      <c r="C37">
+        <v>18.040872310809</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>127</v>
+      </c>
+      <c r="B38">
+        <v>1778889.247211</v>
+      </c>
+      <c r="C38">
+        <v>19.819761558019998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>128</v>
+      </c>
+      <c r="B39">
+        <v>1928308.8708589999</v>
+      </c>
+      <c r="C39">
+        <v>21.748070428879</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>129</v>
+      </c>
+      <c r="B40">
+        <v>2070655.376227</v>
+      </c>
+      <c r="C40">
+        <v>23.818725805105998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>130</v>
+      </c>
+      <c r="B41">
+        <v>2210349.462241</v>
+      </c>
+      <c r="C41">
+        <v>26.029075267347</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>131</v>
+      </c>
+      <c r="B42">
+        <v>2383640.86008</v>
+      </c>
+      <c r="C42">
+        <v>28.412716127427998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>132</v>
+      </c>
+      <c r="B43">
+        <v>2533944.6235130001</v>
+      </c>
+      <c r="C43">
+        <v>30.946660750939998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>133</v>
+      </c>
+      <c r="B44">
+        <v>2695742.2041489999</v>
+      </c>
+      <c r="C44">
+        <v>33.642402955089004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>134</v>
+      </c>
+      <c r="B45">
+        <v>2856655.645</v>
+      </c>
+      <c r="C45">
+        <v>36.499058600089</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>135</v>
+      </c>
+      <c r="B46">
+        <v>3021105.6449910002</v>
+      </c>
+      <c r="C46">
+        <v>39.520164245080004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>136</v>
+      </c>
+      <c r="B47">
+        <v>3212963.9783129999</v>
+      </c>
+      <c r="C47" s="4">
+        <v>42.733128223393003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>137</v>
+      </c>
+      <c r="B48">
+        <v>3405706.4514210001</v>
+      </c>
+      <c r="C48" s="4">
+        <v>46.138834674813005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>138</v>
+      </c>
+      <c r="B49">
+        <v>3594028.2256029998</v>
+      </c>
+      <c r="C49" s="4">
+        <v>49.732862900416997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>139</v>
+      </c>
+      <c r="B50">
+        <v>3801801.0750540001</v>
+      </c>
+      <c r="C50" s="4">
+        <v>53.534663975470998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>140</v>
+      </c>
+      <c r="B51">
+        <v>4036982.2578369998</v>
+      </c>
+      <c r="C51" s="4">
+        <v>57.571646233308002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>141</v>
+      </c>
+      <c r="B52">
+        <v>4255364.7847060002</v>
+      </c>
+      <c r="C52">
+        <v>61.827011018013003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>142</v>
+      </c>
+      <c r="B53">
+        <v>4485241.1287789997</v>
+      </c>
+      <c r="C53">
+        <v>66.312252146792005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>143</v>
+      </c>
+      <c r="B54">
+        <v>4725727.1502710003</v>
+      </c>
+      <c r="C54">
+        <v>71.037979297062989</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>144</v>
+      </c>
+      <c r="B55">
+        <v>4987432.5266000004</v>
+      </c>
+      <c r="C55">
+        <v>76.025411823662992</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>145</v>
+      </c>
+      <c r="B56">
+        <v>5249137.9029289996</v>
+      </c>
+      <c r="C56">
+        <v>81.274549726591999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>146</v>
+      </c>
+      <c r="B57">
+        <v>5530294.3545260001</v>
+      </c>
+      <c r="C57">
+        <v>86.804844081119001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>147</v>
+      </c>
+      <c r="B58">
+        <v>5830901.881391</v>
+      </c>
+      <c r="C58">
+        <v>92.635745962510001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>148</v>
+      </c>
+      <c r="B59">
+        <v>6153612.9028780004</v>
+      </c>
+      <c r="C59">
+        <v>98.78935886538801</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>149</v>
+      </c>
+      <c r="B60">
+        <v>6448915.5910339998</v>
+      </c>
+      <c r="C60">
+        <v>105.238274456422</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>150</v>
+      </c>
+      <c r="B61">
+        <v>6751291.3974679997</v>
+      </c>
+      <c r="C61">
+        <v>111.98956585389</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>151</v>
+      </c>
+      <c r="B62">
+        <v>7068697.5802459996</v>
+      </c>
+      <c r="C62">
+        <v>119.05826343413601</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>152</v>
+      </c>
+      <c r="B63">
+        <v>7367536.8275410002</v>
+      </c>
+      <c r="C63">
+        <v>126.425800261677</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>153</v>
+      </c>
+      <c r="B64">
+        <v>7710583.0640810002</v>
+      </c>
+      <c r="C64">
+        <v>134.13638332575701</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>154</v>
+      </c>
+      <c r="B65">
+        <v>8021800.2683640001</v>
+      </c>
+      <c r="C65">
+        <v>142.15818359412199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>155</v>
+      </c>
+      <c r="B66">
+        <v>8308261.5586710004</v>
+      </c>
+      <c r="C66">
+        <v>150.46644515279201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>156</v>
+      </c>
+      <c r="B67">
+        <v>8585881.4511280004</v>
+      </c>
+      <c r="C67">
+        <v>159.05232660392002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>157</v>
+      </c>
+      <c r="B68">
+        <v>8905055.9134759996</v>
+      </c>
+      <c r="C68">
+        <v>167.95738251739601</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>158</v>
+      </c>
+      <c r="B69">
+        <v>9231303.4941019993</v>
+      </c>
+      <c r="C69">
+        <v>177.18868601149799</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>159</v>
+      </c>
+      <c r="B70">
+        <v>9569929.0317180008</v>
+      </c>
+      <c r="C70">
+        <v>186.758615043215</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>160</v>
+      </c>
+      <c r="B71">
+        <v>9926237.3650310002</v>
+      </c>
+      <c r="C71">
+        <v>196.684852408246</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>161</v>
+      </c>
+      <c r="B72">
+        <v>10276356.71985</v>
+      </c>
+      <c r="C72">
+        <v>206.96120912809602</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>162</v>
+      </c>
+      <c r="B73">
+        <v>10630896.773592999</v>
+      </c>
+      <c r="C73">
+        <v>217.592105901689</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>163</v>
+      </c>
+      <c r="B74">
+        <v>11042021.773569999</v>
+      </c>
+      <c r="C74">
+        <v>228.63412767525898</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>164</v>
+      </c>
+      <c r="B75">
+        <v>11467293.010105001</v>
+      </c>
+      <c r="C75">
+        <v>240.10142068536402</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>165</v>
+      </c>
+      <c r="B76">
+        <v>11907594.622982999</v>
+      </c>
+      <c r="C76">
+        <v>252.00901530834699</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>166</v>
+      </c>
+      <c r="B77">
+        <v>12395639.784246</v>
+      </c>
+      <c r="C77">
+        <v>264.40465509259303</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>167</v>
+      </c>
+      <c r="B78">
+        <v>12881032.526154</v>
+      </c>
+      <c r="C78">
+        <v>277.285687618748</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>168</v>
+      </c>
+      <c r="B79">
+        <v>13377034.945481</v>
+      </c>
+      <c r="C79">
+        <v>290.662722564229</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>169</v>
+      </c>
+      <c r="B80">
+        <v>13934043.009966001</v>
+      </c>
+      <c r="C80">
+        <v>304.59676557419402</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>170</v>
+      </c>
+      <c r="B81">
+        <v>14462758.601334</v>
+      </c>
+      <c r="C81">
+        <v>319.059524175528</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>171</v>
+      </c>
+      <c r="B82">
+        <v>14995010.751840999</v>
+      </c>
+      <c r="C82">
+        <v>334.05453492736899</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>172</v>
+      </c>
+      <c r="B83">
+        <v>15520189.78407</v>
+      </c>
+      <c r="C83">
+        <v>349.57472471143899</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>173</v>
+      </c>
+      <c r="B84">
+        <v>16088691.665758001</v>
+      </c>
+      <c r="C84">
+        <v>365.66341637719705</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>174</v>
+      </c>
+      <c r="B85">
+        <v>16633321.773254</v>
+      </c>
+      <c r="C85">
+        <v>382.29673815045101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>175</v>
+      </c>
+      <c r="B86">
+        <v>17181488.439890001</v>
+      </c>
+      <c r="C86">
+        <v>399.47822659034097</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>176</v>
+      </c>
+      <c r="B87">
+        <v>17749106.181793001</v>
+      </c>
+      <c r="C87">
+        <v>417.22733277213399</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>177</v>
+      </c>
+      <c r="B88">
+        <v>18327333.601115</v>
+      </c>
+      <c r="C88">
+        <v>435.55466637325003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>178</v>
+      </c>
+      <c r="B89">
+        <v>18859585.751623001</v>
+      </c>
+      <c r="C89">
+        <v>454.41425212487297</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>179</v>
+      </c>
+      <c r="B90">
+        <v>19378575.805357002</v>
+      </c>
+      <c r="C90">
+        <v>473.79282793023003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>180</v>
+      </c>
+      <c r="B91">
+        <v>19900218.278446</v>
+      </c>
+      <c r="C91">
+        <v>493.69304620867598</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>181</v>
+      </c>
+      <c r="B92">
+        <v>20469604.299919002</v>
+      </c>
+      <c r="C92">
+        <v>514.16265050859499</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>182</v>
+      </c>
+      <c r="B93">
+        <v>21022191.665479001</v>
+      </c>
+      <c r="C93">
+        <v>535.18484217407399</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>183</v>
+      </c>
+      <c r="B94">
+        <v>21573894.891254999</v>
+      </c>
+      <c r="C94">
+        <v>556.758737065329</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>184</v>
+      </c>
+      <c r="B95">
+        <v>22171573.385845002</v>
+      </c>
+      <c r="C95">
+        <v>578.930310451173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>185</v>
+      </c>
+      <c r="B96">
+        <v>22751569.084736999</v>
+      </c>
+      <c r="C96">
+        <v>601.68187953590996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>186</v>
+      </c>
+      <c r="B97">
+        <v>23351899.998681001</v>
+      </c>
+      <c r="C97">
+        <v>625.03377953459096</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>187</v>
+      </c>
+      <c r="B98">
+        <v>23976986.826602999</v>
+      </c>
+      <c r="C98">
+        <v>649.01076636119399</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>188</v>
+      </c>
+      <c r="B99">
+        <v>24665731.719037</v>
+      </c>
+      <c r="C99">
+        <v>673.676498080231</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>189</v>
+      </c>
+      <c r="B100">
+        <v>25306733.063087001</v>
+      </c>
+      <c r="C100">
+        <v>698.98323114331697</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>190</v>
+      </c>
+      <c r="B101">
+        <v>25970722.041544002</v>
+      </c>
+      <c r="C101">
+        <v>724.95395318486089</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>191</v>
+      </c>
+      <c r="B102">
+        <v>26586083.331831999</v>
+      </c>
+      <c r="C102">
+        <v>751.54003651669302</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>192</v>
+      </c>
+      <c r="B103">
+        <v>27221779.837172002</v>
+      </c>
+      <c r="C103">
+        <v>778.76181635386502</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>193</v>
+      </c>
+      <c r="B104">
+        <v>27853939.783372998</v>
+      </c>
+      <c r="C104">
+        <v>806.61575613723801</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>194</v>
+      </c>
+      <c r="B105">
+        <v>28502014.245701998</v>
+      </c>
+      <c r="C105">
+        <v>835.11777038294008</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>195</v>
+      </c>
+      <c r="B106">
+        <v>29167771.503729001</v>
+      </c>
+      <c r="C106">
+        <v>864.28554188666908</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>196</v>
+      </c>
+      <c r="B107">
+        <v>29828223.923046</v>
+      </c>
+      <c r="C107">
+        <v>894.11376580971603</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>197</v>
+      </c>
+      <c r="B108">
+        <v>30458615.589678001</v>
+      </c>
+      <c r="C108">
+        <v>924.57238139939295</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>198</v>
+      </c>
+      <c r="B109">
+        <v>31088123.116524</v>
+      </c>
+      <c r="C109">
+        <v>955.66050451591695</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>199</v>
+      </c>
+      <c r="B110">
+        <v>31646899.460577998</v>
+      </c>
+      <c r="C110">
+        <v>987.30740397649504</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>200</v>
+      </c>
+      <c r="B111">
+        <v>32234852.417534001</v>
+      </c>
+      <c r="C111">
+        <v>1019.54225639403</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>201</v>
+      </c>
+      <c r="B112">
+        <v>32807774.998147</v>
+      </c>
+      <c r="C112">
+        <v>1052.35003139217</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>202</v>
+      </c>
+      <c r="B113">
+        <v>33388654.836824</v>
+      </c>
+      <c r="C113">
+        <v>1085.738686229</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>203</v>
+      </c>
+      <c r="B114">
+        <v>33992522.309908003</v>
+      </c>
+      <c r="C114">
+        <v>1119.7312085388999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>204</v>
+      </c>
+      <c r="B115">
+        <v>34579591.127079003</v>
+      </c>
+      <c r="C115">
+        <v>1154.3107996659801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>205</v>
+      </c>
+      <c r="B116">
+        <v>35156050.266832002</v>
+      </c>
+      <c r="C116">
+        <v>1189.46684993281</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>206</v>
+      </c>
+      <c r="B117">
+        <v>35698027.954972997</v>
+      </c>
+      <c r="C117">
+        <v>1225.16487788779</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>207</v>
+      </c>
+      <c r="B118">
+        <v>36270066.395801</v>
+      </c>
+      <c r="C118">
+        <v>1261.4349442835901</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>208</v>
+      </c>
+      <c r="B119">
+        <v>36843873.116199002</v>
+      </c>
+      <c r="C119">
+        <v>1298.2788173997901</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>209</v>
+      </c>
+      <c r="B120">
+        <v>37423868.815090999</v>
+      </c>
+      <c r="C120">
+        <v>1335.70268621488</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>210</v>
+      </c>
+      <c r="B121">
+        <v>38002980.374197997</v>
+      </c>
+      <c r="C121">
+        <v>1373.70566658908</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>211</v>
+      </c>
+      <c r="B122">
+        <v>38582976.073090002</v>
+      </c>
+      <c r="C122">
+        <v>1412.2886426621699</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>212</v>
+      </c>
+      <c r="B123">
+        <v>39146173.116068996</v>
+      </c>
+      <c r="C123">
+        <v>1451.4348157782299</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>213</v>
+      </c>
+      <c r="B124">
+        <v>39758881.987002</v>
+      </c>
+      <c r="C124">
+        <v>1491.1936977652399</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>214</v>
+      </c>
+      <c r="B125">
+        <v>40394578.492342003</v>
+      </c>
+      <c r="C125">
+        <v>1531.58827625758</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>215</v>
+      </c>
+      <c r="B126">
+        <v>40981647.309513003</v>
+      </c>
+      <c r="C126">
+        <v>1572.56992356709</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>216</v>
+      </c>
+      <c r="B127">
+        <v>41590819.621307001</v>
+      </c>
+      <c r="C127">
+        <v>1614.1607431883999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>217</v>
+      </c>
+      <c r="B128">
+        <v>42228284.406217001</v>
+      </c>
+      <c r="C128">
+        <v>1656.3890275946201</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>218</v>
+      </c>
+      <c r="B129">
+        <v>42881663.707254998</v>
+      </c>
+      <c r="C129">
+        <v>1699.2706913018701</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>219</v>
+      </c>
+      <c r="B130">
+        <v>43577481.717969</v>
+      </c>
+      <c r="C130">
+        <v>1742.84817301984</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>220</v>
+      </c>
+      <c r="B131">
+        <v>44237049.997501999</v>
+      </c>
+      <c r="C131">
+        <v>1787.08522301734</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>221</v>
+      </c>
+      <c r="B132">
+        <v>44935520.42757</v>
+      </c>
+      <c r="C132">
+        <v>1832.0207434449101</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>222</v>
+      </c>
+      <c r="B133">
+        <v>45622497.040434003</v>
+      </c>
+      <c r="C133">
+        <v>1877.6432404853401</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>223</v>
+      </c>
+      <c r="B134">
+        <v>46381088.975874998</v>
+      </c>
+      <c r="C134">
+        <v>1924.0243294612201</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>224</v>
+      </c>
+      <c r="B135">
+        <v>47119345.696263</v>
+      </c>
+      <c r="C135">
+        <v>1971.1436751574799</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>225</v>
+      </c>
+      <c r="B136">
+        <v>47932754.298367999</v>
+      </c>
+      <c r="C136">
+        <v>2019.0764294558498</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>226</v>
+      </c>
+      <c r="B137">
+        <v>48747047.040257998</v>
+      </c>
+      <c r="C137">
+        <v>2067.8234764961098</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>227</v>
+      </c>
+      <c r="B138">
+        <v>49524205.911181003</v>
+      </c>
+      <c r="C138">
+        <v>2117.34768240729</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>228</v>
+      </c>
+      <c r="B139">
+        <v>50362370.427262999</v>
+      </c>
+      <c r="C139">
+        <v>2167.71005283455</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>229</v>
+      </c>
+      <c r="B140">
+        <v>51163401.072379</v>
+      </c>
+      <c r="C140">
+        <v>2218.8734539069301</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>230</v>
+      </c>
+      <c r="B141">
+        <v>51986535.212118</v>
+      </c>
+      <c r="C141">
+        <v>2270.8599891190502</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>231</v>
+      </c>
+      <c r="B142">
+        <v>52870674.997014001</v>
+      </c>
+      <c r="C142">
+        <v>2323.7306641160599</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>232</v>
+      </c>
+      <c r="B143">
+        <v>53700882.255032003</v>
+      </c>
+      <c r="C143">
+        <v>2377.4315463711</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>233</v>
+      </c>
+      <c r="B144">
+        <v>54510754.297996998</v>
+      </c>
+      <c r="C144">
+        <v>2431.9423006690899</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>234</v>
+      </c>
+      <c r="B145">
+        <v>55337424.996875003</v>
+      </c>
+      <c r="C145">
+        <v>2487.2797256659696</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>235</v>
+      </c>
+      <c r="B146">
+        <v>56142876.340915002</v>
+      </c>
+      <c r="C146">
+        <v>2543.42260200688</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>236</v>
+      </c>
+      <c r="B147">
+        <v>56944791.125816002</v>
+      </c>
+      <c r="C147">
+        <v>2600.3673931326998</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>237</v>
+      </c>
+      <c r="B148">
+        <v>57884631.717161</v>
+      </c>
+      <c r="C148">
+        <v>2658.2520248498604</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>238</v>
+      </c>
+      <c r="B149">
+        <v>58843923.383772999</v>
+      </c>
+      <c r="C149">
+        <v>2717.0959482336302</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>239</v>
+      </c>
+      <c r="B150">
+        <v>59809404.02888</v>
+      </c>
+      <c r="C150">
+        <v>2776.90535226251</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>240</v>
+      </c>
+      <c r="B151">
+        <v>60827933.061081</v>
+      </c>
+      <c r="C151">
+        <v>2837.7332853235898</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>241</v>
+      </c>
+      <c r="B152">
+        <v>61749206.716943003</v>
+      </c>
+      <c r="C152">
+        <v>2899.4824920405404</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>242</v>
+      </c>
+      <c r="B153">
+        <v>62724412.899682999</v>
+      </c>
+      <c r="C153">
+        <v>2962.2069049402198</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>243</v>
+      </c>
+      <c r="B154">
+        <v>63735868.813605003</v>
+      </c>
+      <c r="C154">
+        <v>3025.9427737538199</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>244</v>
+      </c>
+      <c r="B155">
+        <v>64758818.54473</v>
+      </c>
+      <c r="C155">
+        <v>3090.7015922985502</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>245</v>
+      </c>
+      <c r="B156">
+        <v>65831280.103808999</v>
+      </c>
+      <c r="C156">
+        <v>3156.5328724023598</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>246</v>
+      </c>
+      <c r="B157">
+        <v>66939991.394069001</v>
+      </c>
+      <c r="C157">
+        <v>3223.4728637964299</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>247</v>
+      </c>
+      <c r="B158">
+        <v>67986812.899386004</v>
+      </c>
+      <c r="C158">
+        <v>3291.4596766958198</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>248</v>
+      </c>
+      <c r="B159">
+        <v>68972628.759544998</v>
+      </c>
+      <c r="C159">
+        <v>3360.4323054553597</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>249</v>
+      </c>
+      <c r="B160">
+        <v>69999115.049810007</v>
+      </c>
+      <c r="C160">
+        <v>3430.4314205051701</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>250</v>
+      </c>
+      <c r="B161">
+        <v>71030906.178783998</v>
+      </c>
+      <c r="C161">
+        <v>3501.4623266839499</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>251</v>
+      </c>
+      <c r="B162">
+        <v>72162605.103450999</v>
+      </c>
+      <c r="C162">
+        <v>3573.6249317874099</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>252</v>
+      </c>
+      <c r="B163">
+        <v>73296072.307687998</v>
+      </c>
+      <c r="C163">
+        <v>3646.9210040950898</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>253</v>
+      </c>
+      <c r="B164">
+        <v>74396826.339883998</v>
+      </c>
+      <c r="C164">
+        <v>3721.3178304349799</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>254</v>
+      </c>
+      <c r="B165">
+        <v>75594835.748419002</v>
+      </c>
+      <c r="C165">
+        <v>3796.9126661834002</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>255</v>
+      </c>
+      <c r="B166">
+        <v>76740680.909643993</v>
+      </c>
+      <c r="C166">
+        <v>3873.6533470930399</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>256</v>
+      </c>
+      <c r="B167">
+        <v>77938690.318178996</v>
+      </c>
+      <c r="C167">
+        <v>3951.5920374112202</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>257</v>
+      </c>
+      <c r="B168">
+        <v>79149077.683702007</v>
+      </c>
+      <c r="C168">
+        <v>4030.7411150949201</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>258</v>
+      </c>
+      <c r="B169">
+        <v>80342666.393312007</v>
+      </c>
+      <c r="C169">
+        <v>4111.0837814882307</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>259</v>
+      </c>
+      <c r="B170">
+        <v>81600797.307218999</v>
+      </c>
+      <c r="C170">
+        <v>4192.6845787954499</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>260</v>
+      </c>
+      <c r="B171">
+        <v>82898714.511446998</v>
+      </c>
+      <c r="C171">
+        <v>4275.5832933068996</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>261</v>
+      </c>
+      <c r="B172">
+        <v>84203704.833954006</v>
+      </c>
+      <c r="C172">
+        <v>4359.7869981408503</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>262</v>
+      </c>
+      <c r="B173">
+        <v>85416744.618832007</v>
+      </c>
+      <c r="C173">
+        <v>4445.2037427596797</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>263</v>
+      </c>
+      <c r="B174">
+        <v>86666918.274674997</v>
+      </c>
+      <c r="C174">
+        <v>4531.8706610343597</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>264</v>
+      </c>
+      <c r="B175">
+        <v>87928585.747722</v>
+      </c>
+      <c r="C175">
+        <v>4619.7992467820795</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>265</v>
+      </c>
+      <c r="B176">
+        <v>89144277.951954007</v>
+      </c>
+      <c r="C176">
+        <v>4708.9435247340407</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>266</v>
+      </c>
+      <c r="B177">
+        <v>90326372.844361007</v>
+      </c>
+      <c r="C177">
+        <v>4799.2698975783997</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>267</v>
+      </c>
+      <c r="B178">
+        <v>91478406.984081</v>
+      </c>
+      <c r="C178">
+        <v>4890.7483045624804</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>268</v>
+      </c>
+      <c r="B179">
+        <v>92647239.779714003</v>
+      </c>
+      <c r="C179">
+        <v>4983.3955443421901</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>269</v>
+      </c>
+      <c r="B180">
+        <v>93854974.725881994</v>
+      </c>
+      <c r="C180">
+        <v>5077.2505190680704</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>270</v>
+      </c>
+      <c r="B181">
+        <v>95110453.220434994</v>
+      </c>
+      <c r="C181">
+        <v>5172.3609722885103</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>271</v>
+      </c>
+      <c r="B182">
+        <v>96356206.177353993</v>
+      </c>
+      <c r="C182">
+        <v>5268.7171784658603</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>272</v>
+      </c>
+      <c r="B183">
+        <v>97452539.510625005</v>
+      </c>
+      <c r="C183">
+        <v>5366.1697179764897</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>273</v>
+      </c>
+      <c r="B184">
+        <v>98664695.155717999</v>
+      </c>
+      <c r="C184">
+        <v>5464.8344131322001</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>274</v>
+      </c>
+      <c r="B185">
+        <v>99891881.177154005</v>
+      </c>
+      <c r="C185">
+        <v>5564.7262943093592</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>275</v>
+      </c>
+      <c r="B186">
+        <v>101053640.854508</v>
+      </c>
+      <c r="C186">
+        <v>5665.7799351638696</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>276</v>
+      </c>
+      <c r="B187">
+        <v>102242808.86519299</v>
+      </c>
+      <c r="C187">
+        <v>5768.02274402906</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>277</v>
+      </c>
+      <c r="B188">
+        <v>103480604.56404801</v>
+      </c>
+      <c r="C188">
+        <v>5871.5033485931099</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>278</v>
+      </c>
+      <c r="B189">
+        <v>104685687.09086201</v>
+      </c>
+      <c r="C189">
+        <v>5976.1890356839704</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>279</v>
+      </c>
+      <c r="B190">
+        <v>105882812.359611</v>
+      </c>
+      <c r="C190">
+        <v>6082.0718480435798</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>280</v>
+      </c>
+      <c r="B191">
+        <v>107048108.59610499</v>
+      </c>
+      <c r="C191">
+        <v>6189.1199566396799</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>281</v>
+      </c>
+      <c r="B192">
+        <v>108279715.31646501</v>
+      </c>
+      <c r="C192">
+        <v>6297.3996719561501</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>282</v>
+      </c>
+      <c r="B193">
+        <v>109607693.273379</v>
+      </c>
+      <c r="C193">
+        <v>6407.0073652295305</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>283</v>
+      </c>
+      <c r="B194">
+        <v>110891464.24104901</v>
+      </c>
+      <c r="C194">
+        <v>6517.8988294705805</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>284</v>
+      </c>
+      <c r="B195">
+        <v>112157552.41302</v>
+      </c>
+      <c r="C195">
+        <v>6630.0563818835999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>285</v>
+      </c>
+      <c r="B196">
+        <v>113440439.240905</v>
+      </c>
+      <c r="C196">
+        <v>6743.4968211245005</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>286</v>
+      </c>
+      <c r="B197">
+        <v>114774606.176313</v>
+      </c>
+      <c r="C197">
+        <v>6858.2714273008205</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>287</v>
+      </c>
+      <c r="B198">
+        <v>116085785.477314</v>
+      </c>
+      <c r="C198">
+        <v>6974.3572127781299</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>288</v>
+      </c>
+      <c r="B199">
+        <v>117451781.444979</v>
+      </c>
+      <c r="C199">
+        <v>7091.8089942231099</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>289</v>
+      </c>
+      <c r="B200">
+        <v>118831923.649202</v>
+      </c>
+      <c r="C200">
+        <v>7210.6409178723097</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>290</v>
+      </c>
+      <c r="B201">
+        <v>120210297.573856</v>
+      </c>
+      <c r="C201">
+        <v>7330.8512154461696</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>291</v>
+      </c>
+      <c r="B202">
+        <v>121621384.67055</v>
+      </c>
+      <c r="C202">
+        <v>7452.4726001167201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>292</v>
+      </c>
+      <c r="B203">
+        <v>123002411.014558</v>
+      </c>
+      <c r="C203">
+        <v>7575.4750111312796</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>293</v>
+      </c>
+      <c r="B204">
+        <v>124417034.67039201</v>
+      </c>
+      <c r="C204">
+        <v>7699.8920458016701</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>294</v>
+      </c>
+      <c r="B205">
+        <v>126004065.584281</v>
+      </c>
+      <c r="C205">
+        <v>7825.8961113859505</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>295</v>
+      </c>
+      <c r="B206">
+        <v>127437256.175598</v>
+      </c>
+      <c r="C206">
+        <v>7953.3333675615504</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>296</v>
+      </c>
+      <c r="B207">
+        <v>128896970.960462</v>
+      </c>
+      <c r="C207">
+        <v>8082.2303385220102</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>297</v>
+      </c>
+      <c r="B208">
+        <v>130345191.928122</v>
+      </c>
+      <c r="C208">
+        <v>8212.5755304501308</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>298</v>
+      </c>
+      <c r="B209">
+        <v>131819937.089329</v>
+      </c>
+      <c r="C209">
+        <v>8344.3954675394598</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>299</v>
+      </c>
+      <c r="B210">
+        <v>133370718.272037</v>
+      </c>
+      <c r="C210">
+        <v>8477.7661858114989</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>300</v>
+      </c>
+      <c r="B211">
+        <v>134935645.691304</v>
+      </c>
+      <c r="C211">
+        <v>8612.7018315027999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>301</v>
+      </c>
+      <c r="B212">
+        <v>136569536.01379201</v>
+      </c>
+      <c r="C212">
+        <v>8749.2713675165905</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>302</v>
+      </c>
+      <c r="B213">
+        <v>138297145.15347901</v>
+      </c>
+      <c r="C213">
+        <v>8887.56851267007</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>303</v>
+      </c>
+      <c r="B214">
+        <v>140053046.76628301</v>
+      </c>
+      <c r="C214">
+        <v>9027.6215594363603</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>304</v>
+      </c>
+      <c r="B215">
+        <v>141854923.64790201</v>
+      </c>
+      <c r="C215">
+        <v>9169.4764830842614</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>305</v>
+      </c>
+      <c r="B216">
+        <v>143625855.63704899</v>
+      </c>
+      <c r="C216">
+        <v>9313.1023387213099</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>306</v>
+      </c>
+      <c r="B217">
+        <v>145368495.15307999</v>
+      </c>
+      <c r="C217">
+        <v>9458.4708338743894</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>307</v>
+      </c>
+      <c r="B218">
+        <v>147107598.10997099</v>
+      </c>
+      <c r="C218">
+        <v>9605.5784319843606</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>308</v>
+      </c>
+      <c r="B219">
+        <v>148781274.72277999</v>
+      </c>
+      <c r="C219">
+        <v>9754.3597067071405</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>309</v>
+      </c>
+      <c r="B220">
+        <v>150419585.74419299</v>
+      </c>
+      <c r="C220">
+        <v>9904.7792924513305</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>310</v>
+      </c>
+      <c r="B221">
+        <v>152018994.61506999</v>
+      </c>
+      <c r="C221">
+        <v>10056.7982870664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>